<commit_message>
Edits to app, input and dynamic_helper to accommodate the financial scheme description and explanations.
</commit_message>
<xml_diff>
--- a/data/AF_Financial_Scheme.xlsx
+++ b/data/AF_Financial_Scheme.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prajna\Documents\HORTIBONN\PROJECTS\REFOREST\from_partners\EMEA\DA_model\AFDAtool_EMEA_Financial_Scheme\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04093C33-93B6-4299-B71C-9AB25C55516B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E56DC5-1C9D-48BB-9018-583D9FFB4593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="815" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="815" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_names" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="351">
   <si>
     <t>variable</t>
   </si>
@@ -674,21 +674,12 @@
     <t>AF1_total_annual_funding_c</t>
   </si>
   <si>
-    <t>Maintenance support</t>
-  </si>
-  <si>
     <t>Annual maintenance support: Lump sum of funds received annually from external sources in order to maintain the agroforestry system [€]</t>
   </si>
   <si>
     <t>selected_percentage_c</t>
   </si>
   <si>
-    <t>unitless</t>
-  </si>
-  <si>
-    <t>Establishment support as a percentage of total investment costs?</t>
-  </si>
-  <si>
     <t>Shall "Percentage investment funded" be applied?</t>
   </si>
   <si>
@@ -696,9 +687,6 @@
   </si>
   <si>
     <t>ratio</t>
-  </si>
-  <si>
-    <t>Establishment support (as a percentage of total investment costs)</t>
   </si>
   <si>
     <t>Percentage investment funded: Funds received only once from external sources, as a proportion of the investment cost [ratio]</t>
@@ -1112,6 +1100,24 @@
   </si>
   <si>
     <t>Interest Rate [%]</t>
+  </si>
+  <si>
+    <t>AF Establishment Loan amount [€ or GBP or local currency]</t>
+  </si>
+  <si>
+    <t>Establishment support as a percentage of total investment costs [%]</t>
+  </si>
+  <si>
+    <t>Establishment support (% of total investment costs)</t>
+  </si>
+  <si>
+    <t>Annual Maintenance support [€/year]</t>
+  </si>
+  <si>
+    <t>Funds invested for positive social and environmental returns.</t>
+  </si>
+  <si>
+    <t>header6</t>
   </si>
 </sst>
 </file>
@@ -1562,10 +1568,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B10" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -1575,10 +1581,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C0A4C84-585F-4989-ACDA-A26FA8E30FDB}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1632,29 +1638,29 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="H2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="F3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="H3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="H4" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -1666,13 +1672,13 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F5" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="G5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="H5" t="s">
         <v>160</v>
@@ -1681,12 +1687,12 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -1698,10 +1704,10 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="G6" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="H6" t="s">
         <v>160</v>
@@ -1710,12 +1716,12 @@
         <v>0.5</v>
       </c>
       <c r="J6" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -1730,10 +1736,10 @@
         <v>146</v>
       </c>
       <c r="F7" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="G7" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="H7" t="s">
         <v>160</v>
@@ -1742,118 +1748,96 @@
         <v>0.5</v>
       </c>
       <c r="J7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="H8" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="F9" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="H9" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
+      <c r="F10" t="s">
+        <v>349</v>
+      </c>
       <c r="H10" t="s">
-        <v>306</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>322</v>
-      </c>
-      <c r="B11" s="1">
-        <v>100</v>
-      </c>
-      <c r="C11" s="1">
-        <v>50000</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>166</v>
-      </c>
-      <c r="F11" t="s">
-        <v>321</v>
-      </c>
-      <c r="G11" t="s">
-        <v>310</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
       <c r="H11" t="s">
-        <v>160</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>50000</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="F12" t="s">
-        <v>348</v>
+        <v>317</v>
       </c>
       <c r="G12" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="H12" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>325</v>
+        <v>146</v>
       </c>
       <c r="F13" t="s">
-        <v>324</v>
+        <v>344</v>
       </c>
       <c r="G13" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="H13" t="s">
         <v>151</v>
@@ -1862,14 +1846,46 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" t="s">
+        <v>323</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>321</v>
+      </c>
+      <c r="F14" t="s">
+        <v>320</v>
+      </c>
+      <c r="G14" t="s">
+        <v>308</v>
+      </c>
       <c r="H14" t="s">
-        <v>304</v>
+        <v>151</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="H15" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -1947,7 +1963,7 @@
         <v>145</v>
       </c>
       <c r="F2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="H2" t="s">
         <v>151</v>
@@ -1956,7 +1972,7 @@
         <v>1000</v>
       </c>
       <c r="J2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1988,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2017,7 +2033,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2046,7 +2062,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -2066,7 +2082,7 @@
         <v>149</v>
       </c>
       <c r="F6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G6" t="s">
         <v>150</v>
@@ -2078,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2162,7 +2178,7 @@
         <v>0.1</v>
       </c>
       <c r="J2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2179,7 +2195,7 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H3" t="s">
         <v>151</v>
@@ -2188,7 +2204,7 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2214,7 +2230,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2243,7 +2259,7 @@
         <v>0.01</v>
       </c>
       <c r="J5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -2272,7 +2288,7 @@
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -2292,7 +2308,7 @@
         <v>183</v>
       </c>
       <c r="F7" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="H7" t="s">
         <v>160</v>
@@ -2301,7 +2317,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -2330,7 +2346,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -2359,7 +2375,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2388,7 +2404,7 @@
         <v>0.1</v>
       </c>
       <c r="J10" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2417,7 +2433,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="J11" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -2446,7 +2462,7 @@
         <v>100</v>
       </c>
       <c r="J12" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2475,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2504,7 +2520,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2533,7 +2549,7 @@
         <v>0.1</v>
       </c>
       <c r="J15" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2562,7 +2578,7 @@
         <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -2636,7 +2652,7 @@
         <v>197</v>
       </c>
       <c r="F2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
@@ -2645,7 +2661,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2665,7 +2681,7 @@
         <v>197</v>
       </c>
       <c r="F3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H3" t="s">
         <v>160</v>
@@ -2674,7 +2690,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2694,7 +2710,7 @@
         <v>197</v>
       </c>
       <c r="F4" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="H4" t="s">
         <v>160</v>
@@ -2703,7 +2719,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2723,7 +2739,7 @@
         <v>197</v>
       </c>
       <c r="F5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="H5" t="s">
         <v>160</v>
@@ -2732,7 +2748,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -2752,7 +2768,7 @@
         <v>198</v>
       </c>
       <c r="F6" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H6" t="s">
         <v>160</v>
@@ -2761,7 +2777,7 @@
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -2781,7 +2797,7 @@
         <v>200</v>
       </c>
       <c r="F7" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="H7" t="s">
         <v>160</v>
@@ -2790,7 +2806,7 @@
         <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -2819,7 +2835,7 @@
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -2839,7 +2855,7 @@
         <v>198</v>
       </c>
       <c r="F9" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H9" t="s">
         <v>160</v>
@@ -2848,7 +2864,7 @@
         <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2868,7 +2884,7 @@
         <v>198</v>
       </c>
       <c r="F10" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="H10" t="s">
         <v>160</v>
@@ -2877,7 +2893,7 @@
         <v>10</v>
       </c>
       <c r="J10" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2897,7 +2913,7 @@
         <v>198</v>
       </c>
       <c r="F11" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="H11" t="s">
         <v>160</v>
@@ -2906,7 +2922,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -2926,7 +2942,7 @@
         <v>198</v>
       </c>
       <c r="F12" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H12" t="s">
         <v>160</v>
@@ -2935,7 +2951,7 @@
         <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2955,7 +2971,7 @@
         <v>200</v>
       </c>
       <c r="F13" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H13" t="s">
         <v>160</v>
@@ -2964,7 +2980,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2984,7 +3000,7 @@
         <v>198</v>
       </c>
       <c r="F14" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H14" t="s">
         <v>160</v>
@@ -2993,7 +3009,7 @@
         <v>10</v>
       </c>
       <c r="J14" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -3013,7 +3029,7 @@
         <v>198</v>
       </c>
       <c r="F15" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="H15" t="s">
         <v>160</v>
@@ -3022,7 +3038,7 @@
         <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -3042,7 +3058,7 @@
         <v>198</v>
       </c>
       <c r="F16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H16" t="s">
         <v>160</v>
@@ -3051,7 +3067,7 @@
         <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -3071,7 +3087,7 @@
         <v>198</v>
       </c>
       <c r="F17" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H17" t="s">
         <v>160</v>
@@ -3080,7 +3096,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -3100,7 +3116,7 @@
         <v>198</v>
       </c>
       <c r="F18" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H18" t="s">
         <v>160</v>
@@ -3109,7 +3125,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -3129,7 +3145,7 @@
         <v>200</v>
       </c>
       <c r="F19" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="H19" t="s">
         <v>160</v>
@@ -3138,7 +3154,7 @@
         <v>10</v>
       </c>
       <c r="J19" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -3158,7 +3174,7 @@
         <v>198</v>
       </c>
       <c r="F20" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="H20" t="s">
         <v>160</v>
@@ -3167,7 +3183,7 @@
         <v>10</v>
       </c>
       <c r="J20" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -3187,7 +3203,7 @@
         <v>198</v>
       </c>
       <c r="F21" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="H21" t="s">
         <v>160</v>
@@ -3196,7 +3212,7 @@
         <v>10</v>
       </c>
       <c r="J21" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -3216,7 +3232,7 @@
         <v>198</v>
       </c>
       <c r="F22" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="H22" t="s">
         <v>160</v>
@@ -3225,7 +3241,7 @@
         <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -3245,7 +3261,7 @@
         <v>198</v>
       </c>
       <c r="F23" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H23" t="s">
         <v>160</v>
@@ -3254,7 +3270,7 @@
         <v>5</v>
       </c>
       <c r="J23" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -3274,7 +3290,7 @@
         <v>198</v>
       </c>
       <c r="F24" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H24" t="s">
         <v>160</v>
@@ -3283,7 +3299,7 @@
         <v>10</v>
       </c>
       <c r="J24" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -3303,7 +3319,7 @@
         <v>200</v>
       </c>
       <c r="F25" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="H25" t="s">
         <v>160</v>
@@ -3312,7 +3328,7 @@
         <v>10</v>
       </c>
       <c r="J25" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -3332,7 +3348,7 @@
         <v>198</v>
       </c>
       <c r="F26" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="H26" t="s">
         <v>160</v>
@@ -3341,7 +3357,7 @@
         <v>10</v>
       </c>
       <c r="J26" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -3361,7 +3377,7 @@
         <v>198</v>
       </c>
       <c r="F27" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="H27" t="s">
         <v>160</v>
@@ -3370,7 +3386,7 @@
         <v>10</v>
       </c>
       <c r="J27" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -3390,7 +3406,7 @@
         <v>198</v>
       </c>
       <c r="F28" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="H28" t="s">
         <v>160</v>
@@ -3399,7 +3415,7 @@
         <v>10</v>
       </c>
       <c r="J28" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -3419,7 +3435,7 @@
         <v>198</v>
       </c>
       <c r="F29" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="H29" t="s">
         <v>160</v>
@@ -3428,7 +3444,7 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -3440,13 +3456,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D887141-305C-4556-91D4-D86C0CE94422}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.21875" customWidth="1"/>
     <col min="6" max="6" width="94.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3511,7 +3527,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3540,12 +3556,12 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B4" s="3">
         <v>50</v>
@@ -3560,16 +3576,16 @@
         <v>166</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3598,7 +3614,7 @@
         <v>5</v>
       </c>
       <c r="J5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3627,7 +3643,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -3656,7 +3672,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -3685,7 +3701,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3714,7 +3730,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3743,7 +3759,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3772,7 +3788,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -3801,7 +3817,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -3874,7 +3890,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H2" t="s">
         <v>160</v>
@@ -3883,7 +3899,7 @@
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -3909,7 +3925,7 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -3935,7 +3951,7 @@
         <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -3952,7 +3968,7 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="H5" t="s">
         <v>160</v>
@@ -3961,7 +3977,7 @@
         <v>0.01</v>
       </c>
       <c r="J5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -3978,7 +3994,7 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="H6" t="s">
         <v>160</v>
@@ -3987,7 +4003,7 @@
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -4004,7 +4020,7 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="H7" t="s">
         <v>160</v>
@@ -4013,7 +4029,7 @@
         <v>0.1</v>
       </c>
       <c r="J7" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -4030,7 +4046,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H8" t="s">
         <v>160</v>
@@ -4039,7 +4055,7 @@
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -4065,7 +4081,7 @@
         <v>0.5</v>
       </c>
       <c r="J9" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -4091,7 +4107,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -4108,7 +4124,7 @@
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="H11" t="s">
         <v>151</v>
@@ -4117,7 +4133,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -4134,7 +4150,7 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="H12" t="s">
         <v>151</v>
@@ -4143,7 +4159,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -4163,7 +4179,7 @@
         <v>146</v>
       </c>
       <c r="F13" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="H13" t="s">
         <v>160</v>
@@ -4172,7 +4188,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -4189,7 +4205,7 @@
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="H14" t="s">
         <v>151</v>
@@ -4198,7 +4214,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -4215,7 +4231,7 @@
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="H15" t="s">
         <v>151</v>
@@ -4224,7 +4240,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -4241,7 +4257,7 @@
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="H16" t="s">
         <v>160</v>
@@ -4250,7 +4266,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -4267,7 +4283,7 @@
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="H17" t="s">
         <v>160</v>
@@ -4276,7 +4292,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -4293,7 +4309,7 @@
         <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="H18" t="s">
         <v>160</v>
@@ -4302,7 +4318,7 @@
         <v>0.01</v>
       </c>
       <c r="J18" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -4322,7 +4338,7 @@
         <v>146</v>
       </c>
       <c r="F19" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="H19" t="s">
         <v>160</v>
@@ -4331,7 +4347,7 @@
         <v>0.01</v>
       </c>
       <c r="J19" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -4348,7 +4364,7 @@
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="H20" t="s">
         <v>160</v>
@@ -4357,7 +4373,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -4374,7 +4390,7 @@
         <v>7</v>
       </c>
       <c r="F21" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="H21" t="s">
         <v>160</v>
@@ -4383,7 +4399,7 @@
         <v>0.5</v>
       </c>
       <c r="J21" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -4403,7 +4419,7 @@
         <v>171</v>
       </c>
       <c r="F22" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="H22" t="s">
         <v>160</v>
@@ -4412,7 +4428,7 @@
         <v>0.01</v>
       </c>
       <c r="J22" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -4429,7 +4445,7 @@
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="H23" t="s">
         <v>160</v>
@@ -4438,7 +4454,7 @@
         <v>5</v>
       </c>
       <c r="J23" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -4455,7 +4471,7 @@
         <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="H24" t="s">
         <v>160</v>
@@ -4464,7 +4480,7 @@
         <v>5</v>
       </c>
       <c r="J24" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -4536,7 +4552,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>161</v>
@@ -4548,7 +4564,7 @@
         <v>0.01</v>
       </c>
       <c r="J2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -4565,7 +4581,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="H3" t="s">
         <v>160</v>
@@ -4574,7 +4590,7 @@
         <v>1E-3</v>
       </c>
       <c r="J3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -4600,7 +4616,7 @@
         <v>1E-3</v>
       </c>
       <c r="J4" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -4617,7 +4633,7 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="H5" t="s">
         <v>160</v>
@@ -4626,7 +4642,7 @@
         <v>0.01</v>
       </c>
       <c r="J5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -4652,7 +4668,7 @@
         <v>0.01</v>
       </c>
       <c r="J6" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -4681,7 +4697,7 @@
         <v>0.01</v>
       </c>
       <c r="J7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -4698,7 +4714,7 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="H8" t="s">
         <v>151</v>
@@ -4707,7 +4723,7 @@
         <v>0.01</v>
       </c>
       <c r="J8" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -4724,7 +4740,7 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="H9" t="s">
         <v>160</v>
@@ -4733,7 +4749,7 @@
         <v>0.01</v>
       </c>
       <c r="J9" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -4750,7 +4766,7 @@
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="H10" t="s">
         <v>151</v>
@@ -4759,7 +4775,7 @@
         <v>0.01</v>
       </c>
       <c r="J10" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -4776,7 +4792,7 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="H11" t="s">
         <v>160</v>
@@ -4785,7 +4801,7 @@
         <v>0.01</v>
       </c>
       <c r="J11" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -4799,7 +4815,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4845,13 +4861,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B2">
-        <v>9.6</v>
+        <v>14.5</v>
       </c>
       <c r="C2">
-        <v>9.6</v>
+        <v>14.5</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -4860,7 +4876,7 @@
         <v>146</v>
       </c>
       <c r="F2" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="H2" t="s">
         <v>151</v>
@@ -4874,13 +4890,13 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B3">
-        <v>24.6</v>
+        <v>25.4</v>
       </c>
       <c r="C3">
-        <v>24.6</v>
+        <v>25.4</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -4889,7 +4905,7 @@
         <v>146</v>
       </c>
       <c r="F3" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="H3" t="s">
         <v>151</v>
@@ -4903,13 +4919,13 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B4">
-        <v>44.72</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>44.72</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -4918,7 +4934,7 @@
         <v>146</v>
       </c>
       <c r="F4" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="H4" t="s">
         <v>151</v>
@@ -4932,13 +4948,13 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B5">
-        <v>7.23</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="C5">
-        <v>7.23</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -4947,7 +4963,7 @@
         <v>146</v>
       </c>
       <c r="F5" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="H5" t="s">
         <v>151</v>
@@ -4961,13 +4977,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B6">
-        <v>23.15</v>
+        <v>20.059999999999999</v>
       </c>
       <c r="C6">
-        <v>23.15</v>
+        <v>20.059999999999999</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -4976,7 +4992,7 @@
         <v>146</v>
       </c>
       <c r="F6" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="H6" t="s">
         <v>151</v>
@@ -4990,13 +5006,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>23.82</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>23.82</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -5005,7 +5021,7 @@
         <v>146</v>
       </c>
       <c r="F7" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="H7" t="s">
         <v>151</v>
@@ -5019,13 +5035,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B8">
-        <v>23.1</v>
+        <v>19.84</v>
       </c>
       <c r="C8">
-        <v>23.1</v>
+        <v>19.84</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -5034,7 +5050,7 @@
         <v>146</v>
       </c>
       <c r="F8" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="H8" t="s">
         <v>151</v>
@@ -5048,13 +5064,13 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B9">
-        <v>15.14</v>
+        <v>17.61</v>
       </c>
       <c r="C9">
-        <v>15.14</v>
+        <v>17.61</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -5063,7 +5079,7 @@
         <v>146</v>
       </c>
       <c r="F9" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="H9" t="s">
         <v>151</v>
@@ -5077,13 +5093,13 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B10">
-        <v>14.5</v>
+        <v>9.6</v>
       </c>
       <c r="C10">
-        <v>14.5</v>
+        <v>9.6</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -5092,7 +5108,7 @@
         <v>146</v>
       </c>
       <c r="F10" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="H10" t="s">
         <v>151</v>
@@ -5106,13 +5122,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B11">
-        <v>25.4</v>
+        <v>24.6</v>
       </c>
       <c r="C11">
-        <v>25.4</v>
+        <v>24.6</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -5121,7 +5137,7 @@
         <v>146</v>
       </c>
       <c r="F11" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H11" t="s">
         <v>151</v>
@@ -5135,13 +5151,13 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>44.72</v>
       </c>
       <c r="C12">
-        <v>12</v>
+        <v>44.72</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -5150,7 +5166,7 @@
         <v>146</v>
       </c>
       <c r="F12" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="H12" t="s">
         <v>151</v>
@@ -5164,13 +5180,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B13">
-        <v>17.600000000000001</v>
+        <v>7.23</v>
       </c>
       <c r="C13">
-        <v>17.600000000000001</v>
+        <v>7.23</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -5179,7 +5195,7 @@
         <v>146</v>
       </c>
       <c r="F13" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="H13" t="s">
         <v>151</v>
@@ -5193,13 +5209,13 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B14">
-        <v>20.059999999999999</v>
+        <v>23.15</v>
       </c>
       <c r="C14">
-        <v>20.059999999999999</v>
+        <v>23.15</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -5208,7 +5224,7 @@
         <v>146</v>
       </c>
       <c r="F14" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="H14" t="s">
         <v>151</v>
@@ -5222,13 +5238,13 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B15">
-        <v>23.82</v>
+        <v>11</v>
       </c>
       <c r="C15">
-        <v>23.82</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -5237,7 +5253,7 @@
         <v>146</v>
       </c>
       <c r="F15" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="H15" t="s">
         <v>151</v>
@@ -5251,13 +5267,13 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B16">
-        <v>19.84</v>
+        <v>23.1</v>
       </c>
       <c r="C16">
-        <v>19.84</v>
+        <v>23.1</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -5266,7 +5282,7 @@
         <v>146</v>
       </c>
       <c r="F16" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="H16" t="s">
         <v>151</v>
@@ -5280,13 +5296,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B17">
-        <v>17.61</v>
+        <v>15.14</v>
       </c>
       <c r="C17">
-        <v>17.61</v>
+        <v>15.14</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
@@ -5295,7 +5311,7 @@
         <v>146</v>
       </c>
       <c r="F17" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="H17" t="s">
         <v>151</v>
@@ -5324,7 +5340,7 @@
         <v>146</v>
       </c>
       <c r="F18" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="H18" t="s">
         <v>151</v>
@@ -5353,7 +5369,7 @@
         <v>146</v>
       </c>
       <c r="F19" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="H19" t="s">
         <v>151</v>
@@ -5382,7 +5398,7 @@
         <v>146</v>
       </c>
       <c r="F20" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="H20" t="s">
         <v>151</v>
@@ -5411,7 +5427,7 @@
         <v>146</v>
       </c>
       <c r="F21" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="H21" t="s">
         <v>151</v>
@@ -5440,7 +5456,7 @@
         <v>146</v>
       </c>
       <c r="F22" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="H22" t="s">
         <v>151</v>
@@ -5469,7 +5485,7 @@
         <v>146</v>
       </c>
       <c r="F23" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="H23" t="s">
         <v>151</v>
@@ -5498,7 +5514,7 @@
         <v>146</v>
       </c>
       <c r="F24" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="H24" t="s">
         <v>151</v>
@@ -5527,7 +5543,7 @@
         <v>146</v>
       </c>
       <c r="F25" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="H25" t="s">
         <v>151</v>
@@ -5556,7 +5572,7 @@
         <v>146</v>
       </c>
       <c r="F26" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="H26" t="s">
         <v>151</v>
@@ -5585,7 +5601,7 @@
         <v>146</v>
       </c>
       <c r="F27" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H27" t="s">
         <v>151</v>
@@ -5614,7 +5630,7 @@
         <v>146</v>
       </c>
       <c r="F28" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="H28" t="s">
         <v>151</v>
@@ -5643,7 +5659,7 @@
         <v>146</v>
       </c>
       <c r="F29" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="H29" t="s">
         <v>151</v>
@@ -5672,7 +5688,7 @@
         <v>146</v>
       </c>
       <c r="F30" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="H30" t="s">
         <v>151</v>
@@ -5701,7 +5717,7 @@
         <v>146</v>
       </c>
       <c r="F31" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="H31" t="s">
         <v>151</v>
@@ -5730,7 +5746,7 @@
         <v>146</v>
       </c>
       <c r="F32" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="H32" t="s">
         <v>151</v>
@@ -5759,7 +5775,7 @@
         <v>146</v>
       </c>
       <c r="F33" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="H33" t="s">
         <v>151</v>
@@ -5781,8 +5797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21909002-3FEB-40D1-A6BE-6D67D597F061}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5830,57 +5846,51 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>343</v>
       </c>
       <c r="B2" s="1">
-        <v>378</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1">
-        <v>378</v>
+        <v>50000</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>166</v>
       </c>
       <c r="F2" t="s">
-        <v>210</v>
-      </c>
-      <c r="G2" t="s">
-        <v>211</v>
+        <v>345</v>
       </c>
       <c r="H2" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>342</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>213</v>
+        <v>146</v>
       </c>
       <c r="F3" t="s">
-        <v>214</v>
-      </c>
-      <c r="G3" t="s">
-        <v>215</v>
+        <v>344</v>
       </c>
       <c r="H3" t="s">
         <v>151</v>
@@ -5889,62 +5899,62 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B4" s="1">
-        <v>0.75</v>
+        <v>378</v>
       </c>
       <c r="C4" s="1">
-        <v>0.75</v>
+        <v>378</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>217</v>
+        <v>166</v>
       </c>
       <c r="F4" t="s">
-        <v>218</v>
+        <v>348</v>
       </c>
       <c r="G4" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="H4" t="s">
         <v>151</v>
       </c>
       <c r="I4">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="F5" t="s">
-        <v>221</v>
+        <v>346</v>
       </c>
       <c r="G5" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="H5" t="s">
         <v>151</v>
@@ -5953,62 +5963,62 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F6" t="s">
         <v>347</v>
       </c>
-      <c r="B6" s="1">
-        <v>100</v>
-      </c>
-      <c r="C6" s="1">
-        <v>50000</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>166</v>
-      </c>
-      <c r="F6" t="s">
-        <v>321</v>
-      </c>
       <c r="G6" t="s">
-        <v>310</v>
+        <v>215</v>
       </c>
       <c r="H6" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>1E-3</v>
       </c>
       <c r="J6" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>346</v>
+        <v>216</v>
       </c>
       <c r="B7" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="F7" t="s">
-        <v>348</v>
+        <v>217</v>
       </c>
       <c r="G7" t="s">
-        <v>311</v>
+        <v>218</v>
       </c>
       <c r="H7" t="s">
         <v>151</v>
@@ -6017,7 +6027,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>